<commit_message>
version 1.2 add 'everywhere' state
</commit_message>
<xml_diff>
--- a/output/excelFile-1.xlsx
+++ b/output/excelFile-1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>num.</t>
   </si>
@@ -64,33 +64,6 @@
   </si>
   <si>
     <t>comment</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>The Marker</t>
-  </si>
-  <si>
-    <t>https://www.themarker.com/wallstreet/1.5827849</t>
-  </si>
-  <si>
-    <t>19.02.2018 11:17</t>
-  </si>
-  <si>
-    <t>ניו יורק טיימס</t>
-  </si>
-  <si>
-    <t>376</t>
-  </si>
-  <si>
-    <t>הטיול להודו: טראמפ הבן מקים מגדלי יוקרה - האב מטפח את הקשר האסטרטגי</t>
-  </si>
-  <si>
-    <t>דונלד טראמפ הבן, בנו הבכור של נשיא ארה"ב, יגיע השבוע להודו לקידום פרויקטי יוקרה של החברה המשפחתית ■ במקביל, נשיא ארה"ב מקדם את היחסים בין שתי המדינות</t>
-  </si>
-  <si>
-    <t>כאשר המטוס של משפחת טראמפ ינחת השבוע בהודו, האדם שיסייר בדמוקרטיה הגדולה בעולם, בליווי אנשי השירות החשאי, לא יהיה הנשיא שנמצא במשימה דיפלומטית. זה יהיה בנו הבכור, דונלד טראמפ הבן, במסע מכירות.הביקור של בנו של טראמפ נועד לקידום מכירות של דירות יוקרה במיליארד דולר בפרויקט חדש שנבנה כעת בהודו על ידי החברה של טראמפ והשותפים שלה בהודו. הפרויקט מקודם בעיתונים בהודו במודעות שבהן כתוב: "טראמפ הגיע. האם גם אתה הגעת?".לוח הזמנים בביקור של טראמפ הבן כולל מסיבות קוקטייל, ארוחות ערב עם מתווכי נדל"ן, אנשי עסקים ורוכשים פוטנציאלים ומתנהל במקביל לעבודתו של אביו נשיא ארה"ב לחיזוק הקשרים האסטרטגיים בין המדינות.נשיא ארה"ב, שנהנה מתמיכה נרחבת בהודו, קיבל את ראש ממשלת הודו נרנדה מודי בחיבוק חם, כשהאחרון ביקר בוושינגטון ביוני. השניים דנים לעיתים קרובות בהגברת שיתוף הפעולה הצבאי בין שתי המדיניות והגברת המסחר בין המדינות. בנוסף טראמפ אימץ מדיניות קשוחה יותר כלפי סין ופקיסטאן, שתי יריבות של הודו.טראמפ הבן צפוי להגיע היום להודו. משפחת טראמפ הרוויחה 3 מיליון דולר בתמלוגים ב-2016 מיוזמות שקידמה בהודו, כך לפי הדו"חות הכספיים שהגיש הנשיא. איוונקה טראמפ ביקרה בהודו בנובמבר, במסגרת היותה חברה בממשל טראמפ, בדיוק כשמכירות פרויקט הדיור של המשפחה עמדו להתחיל."הרעיון שהבן של הנשיא יקדם פרויקט שנושא את שמו של טראמפ בהודו, כאשר הנשיא דן ביחסים האסטרטגיים בין שתי המדינות הוא פשוט מוזר", אמר דניאל מרקי, שעבד במשרד החוץ של ארה"ב בתיאום מדיניות דרום אסיה במשרד החוץ שלארה"ב בתקופת הנשיאות של ג'ורג' וו. בוש.אין חוק האוסר על טראמפ הבן לפעול לקידום האינטרסים העסקיים שלו – הוא אינו משרת במשרה ציבורית. וגם למרות שהנשיא טראמפ עדיין רשום כנאמן העסקים המשפחתיים, אין מדובר בניגוד עניינים.הודו היא השוק הבינלאומי הגדול ביותר של ארגון טראמפ, עם ארבעה פרויקטים שנבנים בימים אלו. הגדול מבניהם הוא בעיר גורגאון, עיר בקרבת ניו דלהי שצומחת במהירות ומלאה בגורדי שחקים. ארגון טראמפ מקים בעיר שני מגדלים בהם 254 דירות יוקרה, כך לפי החברה.ראג'יב בנסאל, מנהל סוכנות תיווך נדל"ן שמוכרת דירות בפרויקט בגורגאון, אומר כי הקשר הנשיאותי יספיק כדי לעודד את רכישת הדירות. "כולם בהודו יודעים מי זה נשיא ארה"ב. זה סמל סטטוס להיות בעל דירה בבניין שנושא את שמו של הנשיא", הוא אומר.טראמפ הבן אמר בראיון בניו יורק בשבוע שעבר כי הוא טיפח את מערכת היחסים עם הודו במשך עשור וכי רק עכשיו החברה רואה את התוצאות של מאמצים אלו. טראמפ הבן לא ייפגש עם גורמי ממשל בהודו במהלך ביקורו במדינה.</t>
   </si>
 </sst>
 </file>
@@ -179,56 +152,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>